<commit_message>
oa green category takes precedence over bronze
</commit_message>
<xml_diff>
--- a/data/processed/oa_manual.xlsx
+++ b/data/processed/oa_manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vladi\Documents\california-clinical-dashboard\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A71CF8-7C4E-4C42-8EC6-BFB5C10739EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397A301B-2351-4002-8EF2-68927648B4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
   <si>
     <t>doi</t>
-  </si>
-  <si>
-    <t>color_green_only</t>
   </si>
   <si>
     <t>color</t>
@@ -585,27 +582,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="12.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.3671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.734375" customWidth="1"/>
-    <col min="5" max="5" width="12.7890625" customWidth="1"/>
-    <col min="6" max="6" width="44.26171875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.47265625" customWidth="1"/>
-    <col min="8" max="8" width="24.62890625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.734375" customWidth="1"/>
+    <col min="4" max="4" width="12.7890625" customWidth="1"/>
+    <col min="5" max="5" width="44.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.47265625" customWidth="1"/>
+    <col min="7" max="7" width="24.62890625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -622,25 +619,22 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -648,26 +642,23 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="5">
+      <c r="G2" s="5">
         <v>42718</v>
       </c>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -675,31 +666,28 @@
       <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5">
+      <c r="G3" s="5">
         <v>44287</v>
       </c>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -707,26 +695,23 @@
       <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="5">
+        <v>43405</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="5">
-        <v>43405</v>
-      </c>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
@@ -734,58 +719,52 @@
       <c r="F6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+      <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="G9" s="5">
+        <v>42293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="5">
-        <v>42293</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>42</v>
       </c>
       <c r="E10" t="s">
         <v>39</v>
@@ -793,26 +772,23 @@
       <c r="F10" t="s">
         <v>40</v>
       </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="5">
+      <c r="G10" s="5">
         <v>42217</v>
       </c>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
@@ -820,31 +796,28 @@
       <c r="F11" t="s">
         <v>30</v>
       </c>
-      <c r="G11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="5">
+      <c r="G11" s="5">
         <v>41730</v>
       </c>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
+      <c r="B13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
         <v>47</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
       </c>
       <c r="E13" t="s">
         <v>48</v>
@@ -852,52 +825,46 @@
       <c r="F13" t="s">
         <v>49</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="5">
+        <v>42461</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="5">
-        <v>42461</v>
-      </c>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>51</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
         <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" t="s">
-        <v>55</v>
       </c>
       <c r="E14" t="s">
         <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="5">
+        <v>49</v>
+      </c>
+      <c r="G14" s="5">
         <v>43344</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
         <v>56</v>
-      </c>
-      <c r="B15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>14</v>
       </c>
       <c r="E15" t="s">
         <v>57</v>
@@ -905,77 +872,68 @@
       <c r="F15" t="s">
         <v>58</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="5">
+        <v>42510</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="5">
-        <v>42510</v>
-      </c>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
+      <c r="B16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s">
-        <v>14</v>
-      </c>
       <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="5">
+        <v>42278</v>
+      </c>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
         <v>61</v>
       </c>
-      <c r="G16" t="s">
-        <v>59</v>
-      </c>
-      <c r="H16" s="5">
-        <v>42278</v>
-      </c>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
         <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>55</v>
       </c>
       <c r="E17" t="s">
         <v>63</v>
       </c>
       <c r="F17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="5">
+        <v>42942</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
         <v>64</v>
       </c>
-      <c r="G17" t="s">
-        <v>59</v>
-      </c>
-      <c r="H17" s="5">
-        <v>42942</v>
-      </c>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>65</v>
-      </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
         <v>57</v>
@@ -983,13 +941,10 @@
       <c r="F18" t="s">
         <v>58</v>
       </c>
-      <c r="G18" t="s">
-        <v>59</v>
-      </c>
-      <c r="H18" s="5">
+      <c r="G18" s="5">
         <v>43252</v>
       </c>
-      <c r="I18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Mario update Dec 1st 2023
Updates based on https://docs.google.com/document/d/10GnKpvZ1_v9nGDYx3OX5PjW8EyvoaTWszT8e8e24m-c/edit
</commit_message>
<xml_diff>
--- a/data/processed/oa_manual.xlsx
+++ b/data/processed/oa_manual.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vladi\Documents\california-clinical-dashboard\data\processed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\OneDrive\Documents\GitHub\california-clinical-dashboard\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397A301B-2351-4002-8EF2-68927648B4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E2C470-F696-4D83-87E3-40C1EC5A4D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>doi</t>
   </si>
@@ -243,6 +243,21 @@
   </si>
   <si>
     <t>10.1200/jco.2016.34.15_suppl.e14110</t>
+  </si>
+  <si>
+    <t>NCT00780494</t>
+  </si>
+  <si>
+    <t>hybrid</t>
+  </si>
+  <si>
+    <t>NCT01474382</t>
+  </si>
+  <si>
+    <t>NCT02440789</t>
+  </si>
+  <si>
+    <t>NCT02494024</t>
   </si>
 </sst>
 </file>
@@ -303,8 +318,8 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -582,25 +597,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.3671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.734375" customWidth="1"/>
-    <col min="4" max="4" width="12.7890625" customWidth="1"/>
-    <col min="5" max="5" width="44.26171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.47265625" customWidth="1"/>
-    <col min="7" max="7" width="24.62890625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -623,7 +638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -647,7 +662,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -671,12 +686,15 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -700,7 +718,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -720,17 +738,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -753,7 +771,7 @@
         <v>42293</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -777,7 +795,7 @@
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -801,12 +819,12 @@
       </c>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -830,7 +848,7 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -853,7 +871,7 @@
         <v>43344</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -877,7 +895,7 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -898,7 +916,7 @@
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -922,7 +940,7 @@
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -945,6 +963,38 @@
         <v>43252</v>
       </c>
       <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
new pdfs ft screening
</commit_message>
<xml_diff>
--- a/data/processed/oa_manual.xlsx
+++ b/data/processed/oa_manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\OneDrive\Documents\GitHub\california-clinical-dashboard\data\processed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vladi\Documents\california-clinical-dashboard\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E2C470-F696-4D83-87E3-40C1EC5A4D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0C884F-B140-4C73-90D8-9A6A8B06AB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -318,8 +318,8 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -600,22 +600,22 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.68359375" customWidth="1"/>
+    <col min="4" max="4" width="12.83984375" customWidth="1"/>
+    <col min="5" max="5" width="44.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.41796875" customWidth="1"/>
+    <col min="7" max="7" width="24.578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -638,7 +638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -662,7 +662,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -686,7 +686,7 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -694,7 +694,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -718,7 +718,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -738,17 +738,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -771,7 +771,7 @@
         <v>42293</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -795,7 +795,7 @@
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -819,12 +819,12 @@
       </c>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -848,7 +848,7 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -871,7 +871,7 @@
         <v>43344</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -895,7 +895,7 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -916,7 +916,7 @@
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -940,7 +940,7 @@
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -964,7 +964,7 @@
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -972,7 +972,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -980,7 +980,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -988,7 +988,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
new database cleaning step 1
</commit_message>
<xml_diff>
--- a/data/processed/oa_manual.xlsx
+++ b/data/processed/oa_manual.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vladi\Documents\california-clinical-dashboard\data\processed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my_programs\california-clinical-dashboard\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0C884F-B140-4C73-90D8-9A6A8B06AB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="23230" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$22</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
   <si>
     <t>doi</t>
   </si>
@@ -258,12 +260,34 @@
   </si>
   <si>
     <t>NCT02494024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1200/jco.2014.32.3_suppl.115
+</t>
+  </si>
+  <si>
+    <t>10.14283/jpad.2017.36</t>
+  </si>
+  <si>
+    <t>2426-0266</t>
+  </si>
+  <si>
+    <t>Journal of Prevention of Alzheimer's Disease</t>
+  </si>
+  <si>
+    <t>Clinical Trials on Alzheimer’s Disease conference (CTAD)</t>
+  </si>
+  <si>
+    <t>American Society of Clinical Oncology (ASCO)</t>
+  </si>
+  <si>
+    <t>Ovid Technologies (Wolters Kluwer Health)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -281,12 +305,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -302,7 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -316,10 +358,13 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -596,26 +641,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.68359375" customWidth="1"/>
-    <col min="4" max="4" width="12.83984375" customWidth="1"/>
-    <col min="5" max="5" width="44.26171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.41796875" customWidth="1"/>
-    <col min="7" max="7" width="24.578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="44.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="24.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -638,7 +683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -662,7 +707,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -686,7 +731,7 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -694,7 +739,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -718,7 +763,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -738,17 +783,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -771,14 +816,14 @@
         <v>42293</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D10" t="s">
@@ -795,7 +840,7 @@
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -819,12 +864,12 @@
       </c>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -848,14 +893,14 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>50</v>
       </c>
       <c r="B14" t="s">
         <v>51</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D14" t="s">
@@ -871,14 +916,14 @@
         <v>43344</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>55</v>
       </c>
       <c r="B15" t="s">
         <v>68</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D15" t="s">
@@ -888,14 +933,14 @@
         <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="G15" s="5">
         <v>42510</v>
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -916,7 +961,7 @@
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -933,21 +978,21 @@
         <v>63</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="5">
+        <v>80</v>
+      </c>
+      <c r="G17" s="9">
         <v>42942</v>
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>64</v>
       </c>
       <c r="B18" t="s">
         <v>67</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D18" t="s">
@@ -957,14 +1002,14 @@
         <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="5">
+        <v>79</v>
+      </c>
+      <c r="G18" s="9">
         <v>43252</v>
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -972,15 +1017,30 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>69</v>
       </c>
-      <c r="C20" t="s">
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="5">
+        <v>41659</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -988,22 +1048,35 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>73</v>
       </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B16" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{026AA69F-560B-45D3-A33A-84A0FC4D3DBB}"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId2"/>
+    <hyperlink ref="B13" r:id="rId3"/>
+    <hyperlink ref="B16" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated manual xlsx files
</commit_message>
<xml_diff>
--- a/data/processed/oa_manual.xlsx
+++ b/data/processed/oa_manual.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="84">
   <si>
     <t>doi</t>
   </si>
@@ -278,10 +278,19 @@
     <t>Clinical Trials on Alzheimer’s Disease conference (CTAD)</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>American Society of Clinical Oncology (ASCO)</t>
   </si>
   <si>
     <t>Ovid Technologies (Wolters Kluwer Health)</t>
+  </si>
+  <si>
+    <t>Pediatric Dentistry</t>
+  </si>
+  <si>
+    <t>Ingenta</t>
   </si>
 </sst>
 </file>
@@ -645,7 +654,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -933,7 +942,7 @@
         <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G15" s="5">
         <v>42510</v>
@@ -978,7 +987,7 @@
         <v>63</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G17" s="9">
         <v>42942</v>
@@ -1002,7 +1011,7 @@
         <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G18" s="9">
         <v>43252</v>
@@ -1034,7 +1043,7 @@
         <v>57</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G20" s="5">
         <v>41659</v>
@@ -1046,6 +1055,15 @@
       </c>
       <c r="C21" t="s">
         <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>